<commit_message>
correção em comentário de atributo
</commit_message>
<xml_diff>
--- a/Atributos no Autenticação.Gov/Atributos.xlsx
+++ b/Atributos no Autenticação.Gov/Atributos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Atributos" sheetId="1" state="visible" r:id="rId2"/>
@@ -1696,10 +1696,10 @@
   </si>
   <si>
     <t xml:space="preserve">Devolve os atributos profissionais/empresarias/funcionário de qualquer fornecedor registado no SCAP.
-O atributo recebe como parâmetro a lista de fornecedores para os quais se pretende pesquisar atributos (por exemplo http://interop.gov.pt/SCAP?Fornecedor=ANSR,DRE2). Este parâmetro é obrigatório e aceita 1 ou mais valores, desde que separados por ',').
+O atributo recebe como parâmetro a lista de fornecedores para os quais se pretende pesquisar atributos (http://interop.gov.pt/SCAP?Fornecedor=ANSR,DRE2). Este parâmetro é obrigatório e aceita 1 ou mais valores, desde que separados por ',').
 O valor do atributo é devolvido em formato XML. Morada, website e logotipo da entidade só devolvidos para atributos de funcionários e são opcionais.
 * Ver FAScapAttributes.xsd
-* A lista de fornecedores poderá ser consultada na aba Fornecedores SCAP existente neste documento</t>
+* A lista de fornecedores poderá ser consultada na aba Fornecedores SCAP existente neste documento.</t>
   </si>
   <si>
     <t xml:space="preserve">http://interop.gov.pt/MDC/Cidadao/TemAssinaturaDigitalCMD</t>
@@ -2742,7 +2742,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2779,10 +2779,6 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2796,10 +2792,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2891,16 +2883,8 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="15" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2983,10 +2967,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A1:F180" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
   <autoFilter ref="A1:F180">
     <filterColumn colId="4">
-      <filters>
-        <filter val="Disponível"/>
-        <filter val="Planeado"/>
-      </filters>
+      <customFilters and="true">
+        <customFilter operator="equal" val="Disponível"/>
+      </customFilters>
     </filterColumn>
   </autoFilter>
   <tableColumns count="6">
@@ -3007,17 +2990,17 @@
   </sheetPr>
   <dimension ref="A1:G180"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A175" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B177" activeCellId="0" sqref="B177"/>
+      <selection pane="bottomLeft" activeCell="D177" activeCellId="0" sqref="D177"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="53.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="0" width="34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="26.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="49.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="68.85"/>
@@ -3287,10 +3270,10 @@
       <c r="D15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="10" t="s">
+      <c r="E15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9" t="s">
         <v>52</v>
       </c>
     </row>
@@ -3310,7 +3293,7 @@
       <c r="E16" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F16" s="11" t="s">
+      <c r="F16" s="10" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3330,7 +3313,7 @@
       <c r="E17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="F17" s="11" t="s">
         <v>59</v>
       </c>
     </row>
@@ -3350,7 +3333,7 @@
       <c r="E18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="F18" s="11" t="s">
         <v>64</v>
       </c>
     </row>
@@ -3407,7 +3390,7 @@
       <c r="E21" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="12" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3427,7 +3410,7 @@
       <c r="E22" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F22" s="11" t="s">
+      <c r="F22" s="10" t="s">
         <v>81</v>
       </c>
     </row>
@@ -3447,7 +3430,7 @@
       <c r="E23" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="F23" s="11" t="s">
         <v>85</v>
       </c>
     </row>
@@ -3507,7 +3490,7 @@
       <c r="E26" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="F26" s="11" t="s">
         <v>95</v>
       </c>
     </row>
@@ -3607,7 +3590,7 @@
       <c r="E31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F31" s="13" t="s">
+      <c r="F31" s="12" t="s">
         <v>77</v>
       </c>
     </row>
@@ -3615,7 +3598,7 @@
       <c r="A32" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B32" s="9" t="s">
+      <c r="B32" s="4" t="s">
         <v>111</v>
       </c>
       <c r="C32" s="0" t="s">
@@ -3635,7 +3618,7 @@
       <c r="A33" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="9" t="s">
+      <c r="B33" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C33" s="0" t="s">
@@ -3727,7 +3710,7 @@
       <c r="E37" s="0" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="12" t="s">
+      <c r="F37" s="11" t="s">
         <v>124</v>
       </c>
     </row>
@@ -4207,7 +4190,7 @@
       <c r="E61" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F61" s="13" t="s">
+      <c r="F61" s="12" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4227,10 +4210,10 @@
       <c r="E62" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F62" s="13" t="s">
+      <c r="F62" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G62" s="14"/>
+      <c r="G62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
@@ -4248,10 +4231,10 @@
       <c r="E63" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F63" s="13" t="s">
+      <c r="F63" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G63" s="14"/>
+      <c r="G63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
@@ -4269,10 +4252,10 @@
       <c r="E64" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F64" s="13" t="s">
+      <c r="F64" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G64" s="14"/>
+      <c r="G64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="1" t="s">
@@ -4290,10 +4273,10 @@
       <c r="E65" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="13" t="s">
+      <c r="F65" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G65" s="14"/>
+      <c r="G65" s="5"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
@@ -4311,10 +4294,10 @@
       <c r="E66" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F66" s="13" t="s">
+      <c r="F66" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G66" s="14"/>
+      <c r="G66" s="5"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
@@ -4332,10 +4315,10 @@
       <c r="E67" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F67" s="13" t="s">
+      <c r="F67" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G67" s="14"/>
+      <c r="G67" s="5"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
@@ -4353,10 +4336,10 @@
       <c r="E68" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F68" s="13" t="s">
+      <c r="F68" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G68" s="14"/>
+      <c r="G68" s="5"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
@@ -4374,10 +4357,10 @@
       <c r="E69" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F69" s="13" t="s">
+      <c r="F69" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G69" s="14"/>
+      <c r="G69" s="5"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="1" t="s">
@@ -4395,10 +4378,10 @@
       <c r="E70" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F70" s="13" t="s">
+      <c r="F70" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G70" s="14"/>
+      <c r="G70" s="5"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="1" t="s">
@@ -4416,10 +4399,10 @@
       <c r="E71" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F71" s="13" t="s">
+      <c r="F71" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G71" s="14"/>
+      <c r="G71" s="5"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
@@ -4437,10 +4420,10 @@
       <c r="E72" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F72" s="13" t="s">
+      <c r="F72" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G72" s="14"/>
+      <c r="G72" s="5"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
@@ -4458,10 +4441,10 @@
       <c r="E73" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F73" s="13" t="s">
+      <c r="F73" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G73" s="14"/>
+      <c r="G73" s="5"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="1" t="s">
@@ -4479,10 +4462,10 @@
       <c r="E74" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F74" s="13" t="s">
+      <c r="F74" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G74" s="14"/>
+      <c r="G74" s="5"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
@@ -4500,10 +4483,10 @@
       <c r="E75" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F75" s="13" t="s">
+      <c r="F75" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G75" s="14"/>
+      <c r="G75" s="5"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="1" t="s">
@@ -4521,10 +4504,10 @@
       <c r="E76" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F76" s="13" t="s">
+      <c r="F76" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G76" s="14"/>
+      <c r="G76" s="5"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A77" s="1" t="s">
@@ -4542,10 +4525,10 @@
       <c r="E77" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F77" s="13" t="s">
+      <c r="F77" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G77" s="14"/>
+      <c r="G77" s="5"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="1" t="s">
@@ -4563,376 +4546,376 @@
       <c r="E78" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F78" s="13" t="s">
+      <c r="F78" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="G78" s="14"/>
+      <c r="G78" s="5"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="15" t="s">
+      <c r="A79" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="C79" s="15" t="s">
+      <c r="C79" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="D79" s="15" t="s">
+      <c r="D79" s="13" t="s">
         <v>225</v>
       </c>
-      <c r="E79" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F79" s="15" t="s">
+      <c r="E79" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F79" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G79" s="17" t="s">
+      <c r="G79" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="15" t="s">
+      <c r="A80" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B80" s="16" t="s">
+      <c r="B80" s="14" t="s">
         <v>227</v>
       </c>
-      <c r="C80" s="15" t="s">
+      <c r="C80" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="D80" s="15" t="s">
+      <c r="D80" s="13" t="s">
         <v>228</v>
       </c>
-      <c r="E80" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F80" s="15" t="s">
+      <c r="E80" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F80" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G80" s="17" t="s">
+      <c r="G80" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="15" t="s">
+      <c r="A81" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B81" s="16" t="s">
+      <c r="B81" s="14" t="s">
         <v>229</v>
       </c>
-      <c r="C81" s="15" t="s">
+      <c r="C81" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="D81" s="15" t="s">
+      <c r="D81" s="13" t="s">
         <v>230</v>
       </c>
-      <c r="E81" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F81" s="15" t="s">
+      <c r="E81" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F81" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G81" s="17" t="s">
+      <c r="G81" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A82" s="15" t="s">
+      <c r="A82" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B82" s="16" t="s">
+      <c r="B82" s="14" t="s">
         <v>231</v>
       </c>
-      <c r="C82" s="15" t="s">
+      <c r="C82" s="13" t="s">
         <v>232</v>
       </c>
-      <c r="D82" s="15" t="s">
+      <c r="D82" s="13" t="s">
         <v>233</v>
       </c>
-      <c r="E82" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F82" s="15" t="s">
+      <c r="E82" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F82" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G82" s="17" t="s">
+      <c r="G82" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A83" s="15" t="s">
+      <c r="A83" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B83" s="16" t="s">
+      <c r="B83" s="14" t="s">
         <v>234</v>
       </c>
-      <c r="C83" s="15" t="s">
+      <c r="C83" s="13" t="s">
         <v>235</v>
       </c>
-      <c r="D83" s="15" t="s">
+      <c r="D83" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="E83" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F83" s="15" t="s">
+      <c r="E83" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F83" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G83" s="17" t="s">
+      <c r="G83" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="15" t="s">
+      <c r="A84" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="14" t="s">
         <v>237</v>
       </c>
-      <c r="C84" s="15" t="s">
+      <c r="C84" s="13" t="s">
         <v>238</v>
       </c>
-      <c r="D84" s="15" t="s">
+      <c r="D84" s="13" t="s">
         <v>239</v>
       </c>
-      <c r="E84" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F84" s="15" t="s">
+      <c r="E84" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F84" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G84" s="17" t="s">
+      <c r="G84" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="15" t="s">
+      <c r="A85" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B85" s="16" t="s">
+      <c r="B85" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="C85" s="15" t="s">
+      <c r="C85" s="13" t="s">
         <v>241</v>
       </c>
-      <c r="D85" s="15" t="s">
+      <c r="D85" s="13" t="s">
         <v>242</v>
       </c>
-      <c r="E85" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F85" s="15" t="s">
+      <c r="E85" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F85" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G85" s="17" t="s">
+      <c r="G85" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="15" t="s">
+      <c r="A86" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B86" s="16" t="s">
+      <c r="B86" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="C86" s="15" t="s">
+      <c r="C86" s="13" t="s">
         <v>244</v>
       </c>
-      <c r="D86" s="15" t="s">
+      <c r="D86" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="E86" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F86" s="15" t="s">
+      <c r="E86" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F86" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G86" s="17" t="s">
+      <c r="G86" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="15" t="s">
+      <c r="A87" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B87" s="16" t="s">
+      <c r="B87" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="C87" s="15" t="s">
+      <c r="C87" s="13" t="s">
         <v>247</v>
       </c>
-      <c r="D87" s="15" t="s">
+      <c r="D87" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="E87" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F87" s="15" t="s">
+      <c r="E87" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F87" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G87" s="17" t="s">
+      <c r="G87" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="15" t="s">
+      <c r="A88" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B88" s="16" t="s">
+      <c r="B88" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="C88" s="15" t="s">
+      <c r="C88" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="D88" s="15" t="s">
+      <c r="D88" s="13" t="s">
         <v>250</v>
       </c>
-      <c r="E88" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F88" s="15" t="s">
+      <c r="E88" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F88" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G88" s="17" t="s">
+      <c r="G88" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="15" t="s">
+      <c r="A89" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="14" t="s">
         <v>251</v>
       </c>
-      <c r="C89" s="15" t="s">
+      <c r="C89" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="D89" s="15" t="s">
+      <c r="D89" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="E89" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F89" s="15" t="s">
+      <c r="E89" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G89" s="17" t="s">
+      <c r="G89" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="15" t="s">
+      <c r="A90" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B90" s="16" t="s">
+      <c r="B90" s="14" t="s">
         <v>253</v>
       </c>
-      <c r="C90" s="15" t="s">
+      <c r="C90" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="D90" s="15" t="s">
+      <c r="D90" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="E90" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F90" s="15" t="s">
+      <c r="E90" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F90" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G90" s="17" t="s">
+      <c r="G90" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="15" t="s">
+      <c r="A91" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B91" s="16" t="s">
+      <c r="B91" s="14" t="s">
         <v>255</v>
       </c>
-      <c r="C91" s="15" t="s">
+      <c r="C91" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="D91" s="15" t="s">
+      <c r="D91" s="13" t="s">
         <v>256</v>
       </c>
-      <c r="E91" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F91" s="15" t="s">
+      <c r="E91" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F91" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G91" s="17" t="s">
+      <c r="G91" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="15" t="s">
+      <c r="A92" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B92" s="16" t="s">
+      <c r="B92" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="C92" s="13" t="s">
         <v>258</v>
       </c>
-      <c r="D92" s="15" t="s">
+      <c r="D92" s="13" t="s">
         <v>259</v>
       </c>
-      <c r="E92" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F92" s="15" t="s">
+      <c r="E92" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F92" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G92" s="17" t="s">
+      <c r="G92" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="15" t="s">
+      <c r="A93" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B93" s="16" t="s">
+      <c r="B93" s="14" t="s">
         <v>260</v>
       </c>
-      <c r="C93" s="15" t="s">
+      <c r="C93" s="13" t="s">
         <v>261</v>
       </c>
-      <c r="D93" s="15" t="s">
+      <c r="D93" s="13" t="s">
         <v>262</v>
       </c>
-      <c r="E93" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F93" s="15" t="s">
+      <c r="E93" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F93" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G93" s="17" t="s">
+      <c r="G93" s="15" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="15" t="s">
+      <c r="A94" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B94" s="16" t="s">
+      <c r="B94" s="14" t="s">
         <v>263</v>
       </c>
-      <c r="C94" s="15" t="s">
+      <c r="C94" s="13" t="s">
         <v>264</v>
       </c>
-      <c r="D94" s="15" t="s">
+      <c r="D94" s="13" t="s">
         <v>265</v>
       </c>
-      <c r="E94" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F94" s="15" t="s">
+      <c r="E94" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F94" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="G94" s="17" t="s">
+      <c r="G94" s="15" t="s">
         <v>226</v>
       </c>
     </row>
@@ -4952,7 +4935,7 @@
       <c r="E95" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F95" s="13" t="s">
+      <c r="F95" s="12" t="s">
         <v>77</v>
       </c>
     </row>
@@ -4972,7 +4955,7 @@
       <c r="E96" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F96" s="13" t="s">
+      <c r="F96" s="12" t="s">
         <v>77</v>
       </c>
     </row>
@@ -5385,25 +5368,25 @@
       </c>
     </row>
     <row r="121" s="5" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A121" s="9" t="s">
+      <c r="A121" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B121" s="16" t="s">
+      <c r="B121" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="C121" s="15" t="s">
+      <c r="C121" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="D121" s="15" t="s">
+      <c r="D121" s="13" t="s">
         <v>343</v>
       </c>
-      <c r="E121" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="F121" s="15" t="s">
+      <c r="E121" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="F121" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="G121" s="17" t="s">
+      <c r="G121" s="15" t="s">
         <v>345</v>
       </c>
     </row>
@@ -5437,7 +5420,7 @@
       <c r="E123" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F123" s="12" t="s">
+      <c r="F123" s="11" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5457,7 +5440,7 @@
       <c r="E124" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F124" s="12" t="s">
+      <c r="F124" s="11" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5477,7 +5460,7 @@
       <c r="E125" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F125" s="12" t="s">
+      <c r="F125" s="11" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5497,7 +5480,7 @@
       <c r="E126" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F126" s="12" t="s">
+      <c r="F126" s="11" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5517,7 +5500,7 @@
       <c r="E127" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F127" s="12" t="s">
+      <c r="F127" s="11" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5537,7 +5520,7 @@
       <c r="E128" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F128" s="12" t="s">
+      <c r="F128" s="11" t="s">
         <v>353</v>
       </c>
     </row>
@@ -5558,7 +5541,7 @@
         <v>11</v>
       </c>
       <c r="F129" s="5"/>
-      <c r="G129" s="18" t="s">
+      <c r="G129" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5578,7 +5561,7 @@
       <c r="E130" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G130" s="18" t="s">
+      <c r="G130" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5598,10 +5581,10 @@
       <c r="E131" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F131" s="12" t="s">
+      <c r="F131" s="11" t="s">
         <v>373</v>
       </c>
-      <c r="G131" s="18" t="s">
+      <c r="G131" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5622,7 +5605,7 @@
         <v>11</v>
       </c>
       <c r="F132" s="5"/>
-      <c r="G132" s="18" t="s">
+      <c r="G132" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5643,7 +5626,7 @@
         <v>11</v>
       </c>
       <c r="F133" s="5"/>
-      <c r="G133" s="18" t="s">
+      <c r="G133" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5664,7 +5647,7 @@
         <v>11</v>
       </c>
       <c r="F134" s="5"/>
-      <c r="G134" s="18" t="s">
+      <c r="G134" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5684,7 +5667,7 @@
       <c r="E135" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G135" s="18" t="s">
+      <c r="G135" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5705,7 +5688,7 @@
         <v>11</v>
       </c>
       <c r="F136" s="5"/>
-      <c r="G136" s="18" t="s">
+      <c r="G136" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5725,10 +5708,10 @@
       <c r="E137" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F137" s="12" t="s">
+      <c r="F137" s="11" t="s">
         <v>389</v>
       </c>
-      <c r="G137" s="18" t="s">
+      <c r="G137" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5749,7 +5732,7 @@
         <v>11</v>
       </c>
       <c r="F138" s="5"/>
-      <c r="G138" s="18" t="s">
+      <c r="G138" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5770,7 +5753,7 @@
         <v>11</v>
       </c>
       <c r="F139" s="5"/>
-      <c r="G139" s="18" t="s">
+      <c r="G139" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5791,7 +5774,7 @@
         <v>11</v>
       </c>
       <c r="F140" s="5"/>
-      <c r="G140" s="18" t="s">
+      <c r="G140" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5812,7 +5795,7 @@
         <v>11</v>
       </c>
       <c r="F141" s="5"/>
-      <c r="G141" s="18" t="s">
+      <c r="G141" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5833,7 +5816,7 @@
         <v>11</v>
       </c>
       <c r="F142" s="5"/>
-      <c r="G142" s="18" t="s">
+      <c r="G142" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5854,7 +5837,7 @@
         <v>11</v>
       </c>
       <c r="F143" s="5"/>
-      <c r="G143" s="18" t="s">
+      <c r="G143" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5875,7 +5858,7 @@
         <v>11</v>
       </c>
       <c r="F144" s="5"/>
-      <c r="G144" s="18" t="s">
+      <c r="G144" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5896,7 +5879,7 @@
         <v>11</v>
       </c>
       <c r="F145" s="5"/>
-      <c r="G145" s="18" t="s">
+      <c r="G145" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -5916,18 +5899,18 @@
       <c r="E146" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F146" s="12" t="s">
+      <c r="F146" s="11" t="s">
         <v>409</v>
       </c>
-      <c r="G146" s="18" t="s">
+      <c r="G146" s="16" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="147" s="5" customFormat="true" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A147" s="9" t="s">
+      <c r="A147" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B147" s="14" t="s">
+      <c r="B147" s="5" t="s">
         <v>410</v>
       </c>
       <c r="C147" s="5" t="s">
@@ -5939,10 +5922,10 @@
       <c r="E147" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F147" s="12" t="s">
+      <c r="F147" s="11" t="s">
         <v>413</v>
       </c>
-      <c r="G147" s="18" t="s">
+      <c r="G147" s="16" t="s">
         <v>367</v>
       </c>
     </row>
@@ -6322,7 +6305,7 @@
       <c r="E166" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F166" s="12" t="s">
+      <c r="F166" s="11" t="s">
         <v>473</v>
       </c>
     </row>
@@ -6482,7 +6465,7 @@
       <c r="E174" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F174" s="12" t="s">
+      <c r="F174" s="11" t="s">
         <v>499</v>
       </c>
     </row>
@@ -6502,10 +6485,10 @@
       <c r="E175" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F175" s="12" t="s">
+      <c r="F175" s="11" t="s">
         <v>503</v>
       </c>
-      <c r="G175" s="19" t="s">
+      <c r="G175" s="17" t="s">
         <v>504</v>
       </c>
     </row>
@@ -6525,10 +6508,10 @@
       <c r="E176" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F176" s="12" t="s">
+      <c r="F176" s="11" t="s">
         <v>508</v>
       </c>
-      <c r="G176" s="19" t="s">
+      <c r="G176" s="17" t="s">
         <v>504</v>
       </c>
     </row>
@@ -6548,10 +6531,10 @@
       <c r="E177" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F177" s="12" t="s">
+      <c r="F177" s="11" t="s">
         <v>512</v>
       </c>
-      <c r="G177" s="19" t="s">
+      <c r="G177" s="17" t="s">
         <v>504</v>
       </c>
     </row>
@@ -6571,16 +6554,13 @@
       <c r="E178" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="F178" s="12" t="s">
+      <c r="F178" s="11" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="180" customFormat="false" ht="15" hidden="true" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F177" r:id="rId2" display="http://interop"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6588,9 +6568,9 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <legacyDrawing r:id="rId3"/>
+  <legacyDrawing r:id="rId2"/>
   <tableParts>
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6602,13 +6582,13 @@
   </sheetPr>
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="44.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="61.29"/>
@@ -6616,17 +6596,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="74.28"/>
   </cols>
   <sheetData>
-    <row r="1" s="20" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="20" t="s">
+    <row r="1" s="18" customFormat="true" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="18" t="s">
         <v>517</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="18" t="s">
         <v>518</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="18" t="s">
         <v>519</v>
       </c>
     </row>
@@ -6637,7 +6617,7 @@
       <c r="B2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="19" t="s">
         <v>521</v>
       </c>
     </row>
@@ -6648,7 +6628,7 @@
       <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>523</v>
       </c>
     </row>
@@ -6659,7 +6639,7 @@
       <c r="B4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="20" t="s">
         <v>523</v>
       </c>
     </row>
@@ -6670,7 +6650,7 @@
       <c r="B5" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="20" t="s">
         <v>523</v>
       </c>
     </row>
@@ -6692,7 +6672,7 @@
       <c r="B7" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="20" t="s">
         <v>523</v>
       </c>
       <c r="D7" s="5" t="s">
@@ -6706,10 +6686,10 @@
       <c r="B8" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="20" t="s">
         <v>523</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>528</v>
       </c>
     </row>
@@ -6717,10 +6697,10 @@
       <c r="A9" s="0" t="s">
         <v>117</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="20" t="s">
         <v>523</v>
       </c>
       <c r="D9" s="5" t="s">
@@ -6728,16 +6708,16 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="21" t="s">
         <v>530</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="22" t="s">
         <v>531</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="23" t="s">
         <v>532</v>
       </c>
     </row>
@@ -6748,7 +6728,7 @@
       <c r="B11" s="8" t="s">
         <v>467</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="20" t="s">
         <v>523</v>
       </c>
       <c r="D11" s="0" t="s">
@@ -6762,12 +6742,12 @@
       <c r="B12" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="20" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="11" t="s">
         <v>535</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -6795,7 +6775,7 @@
       <c r="B15" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="20" t="s">
         <v>523</v>
       </c>
       <c r="D15" s="5" t="s">
@@ -6809,7 +6789,7 @@
       <c r="B16" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C16" s="22" t="s">
+      <c r="C16" s="20" t="s">
         <v>523</v>
       </c>
       <c r="D16" s="0" t="s">
@@ -6823,7 +6803,7 @@
       <c r="B17" s="4" t="s">
         <v>541</v>
       </c>
-      <c r="C17" s="22" t="s">
+      <c r="C17" s="20" t="s">
         <v>523</v>
       </c>
       <c r="D17" s="0" t="s">
@@ -7048,93 +7028,93 @@
   </sheetPr>
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="89.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="94.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="24" t="s">
         <v>543</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="24" t="s">
         <v>544</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="25" t="s">
         <v>545</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="26" t="s">
         <v>546</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="25" t="s">
         <v>547</v>
       </c>
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="26" t="s">
         <v>548</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="25" t="s">
         <v>549</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="26" t="s">
         <v>550</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="25" t="s">
         <v>551</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="B5" s="26" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="25" t="s">
         <v>553</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="26" t="s">
         <v>554</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="25" t="s">
         <v>555</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="26" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="26" t="s">
         <v>557</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27" t="s">
+      <c r="A9" s="25" t="s">
         <v>558</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="26" t="s">
         <v>559</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="25" t="s">
         <v>560</v>
       </c>
-      <c r="B10" s="28" t="s">
+      <c r="B10" s="26" t="s">
         <v>561</v>
       </c>
     </row>
@@ -7156,209 +7136,209 @@
   </sheetPr>
   <dimension ref="A1:A42"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="253.42"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="27" t="s">
         <v>562</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="30"/>
+      <c r="A2" s="28"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="31" t="s">
+      <c r="A3" s="29" t="s">
         <v>563</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32"/>
+      <c r="A4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="12" t="s">
         <v>564</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="31" t="s">
         <v>565</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="33" t="s">
+      <c r="A7" s="31" t="s">
         <v>566</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="31" t="s">
         <v>567</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="33" t="s">
+      <c r="A9" s="31" t="s">
         <v>568</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="33" t="s">
+      <c r="A10" s="31" t="s">
         <v>569</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="33" t="s">
+      <c r="A11" s="31" t="s">
         <v>570</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="33" t="s">
+      <c r="A12" s="31" t="s">
         <v>571</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="31" t="s">
         <v>572</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="33"/>
+      <c r="A14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="34" t="s">
+      <c r="A15" s="32" t="s">
         <v>573</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="35"/>
+      <c r="A16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="12" t="s">
         <v>574</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
+      <c r="A18" s="34" t="s">
         <v>575</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
+      <c r="A20" s="34" t="s">
         <v>576</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="34" t="s">
         <v>577</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="37" t="s">
+      <c r="A22" s="34" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="37" t="s">
+      <c r="A23" s="34" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="34" t="s">
         <v>578</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="37" t="s">
+      <c r="A25" s="34" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="34" t="s">
         <v>579</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="34" t="s">
         <v>475</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="34" t="s">
         <v>479</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="34" t="s">
         <v>482</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="37" t="s">
+      <c r="A30" s="34" t="s">
         <v>485</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="36"/>
+      <c r="A31" s="34"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="35" t="s">
         <v>580</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="39" t="s">
+      <c r="A33" s="34" t="s">
         <v>581</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="34" t="s">
         <v>582</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="40" t="s">
+      <c r="A35" s="36" t="s">
         <v>583</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="12" t="s">
         <v>584</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="34" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="34" t="s">
         <v>586</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="34" t="s">
         <v>587</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="37" t="s">
+      <c r="A41" s="34" t="s">
         <v>588</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="37"/>
+      <c r="A42" s="34"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Correção de nome e designação.
</commit_message>
<xml_diff>
--- a/Atributos no Autenticação.Gov/Atributos.xlsx
+++ b/Atributos no Autenticação.Gov/Atributos.xlsx
@@ -2014,10 +2014,10 @@
     <t xml:space="preserve">ANSR</t>
   </si>
   <si>
-    <t xml:space="preserve">Diário da República Eletrónico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DRE2</t>
+    <t xml:space="preserve">Diário da República</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRE</t>
   </si>
   <si>
     <t xml:space="preserve">Governo Regional da Madeira</t>
@@ -2960,8 +2960,8 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FFFFFFFF"/>
+          <fgColor rgb="FF3C3C3C"/>
+          <bgColor rgb="FFFCFCFC"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3050,7 +3050,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6642,7 +6642,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6654,7 +6654,7 @@
       <selection pane="bottomLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="44.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="61.3"/>
@@ -7088,17 +7088,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B27" activeCellId="0" sqref="B27"/>
+      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="94.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="31.83"/>
@@ -7220,7 +7220,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -7232,7 +7232,7 @@
       <selection pane="bottomLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="253.42"/>
   </cols>

</xml_diff>